<commit_message>
Doplněný SQL projekt v02 dle feedbacku lektora: - změněn název repozitáře podle projektu - README.md - doplněn popis zadání a odpovědi na otázky - 220322_SQL_Project_LZ_v01 - upraven formát souboru a komentář k výstupům a odpovědím - 220322_Task_5_HDP_vliv_na_mzdy_a_ceny - doplněny intervaly spolehlivosti k lineárním trendům
</commit_message>
<xml_diff>
--- a/SQL_project/220322_Task_5_HDP_vliv_na_mzdy_a_ceny.xlsx
+++ b/SQL_project/220322_Task_5_HDP_vliv_na_mzdy_a_ceny.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AAA_Osobni_new\AAA_Study\22_02_Data_Academy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD527703-8010-497E-B629-0D95E96854A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58E1606A-55F7-4D99-BD77-188BFC7A6BA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-6310" windowWidth="38620" windowHeight="21820" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-29430" yWindow="-4820" windowWidth="17960" windowHeight="10340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vliv_stejny_rok" sheetId="1" r:id="rId1"/>
@@ -753,13 +753,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
+            <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.12130664916885389"/>
-                  <c:y val="8.9865850102070571E-2"/>
+                  <c:x val="0.14669466316710411"/>
+                  <c:y val="7.5660542432195971E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -1215,13 +1215,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
+            <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.13158355205599301"/>
-                  <c:y val="0.11660141440653252"/>
+                  <c:x val="0.1704724409448819"/>
+                  <c:y val="0.10036271507728201"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -1692,7 +1692,7 @@
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
+            <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout>
@@ -2170,12 +2170,26 @@
             </c:spPr>
             <c:trendlineType val="linear"/>
             <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.11340749536259323"/>
-                  <c:y val="7.9841426071741037E-2"/>
+                  <c:x val="9.3949538448069247E-2"/>
+                  <c:y val="0.10526939340915718"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -5226,8 +5240,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5642,9 +5656,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57CC11A3-819E-4334-A5BD-5C7D7A7AE295}">
   <dimension ref="B2:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>